<commit_message>
Update based on deleted test folders
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\1D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876AEA5D-9935-4937-A01F-D1931D71F3A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ECABE4-407B-4852-8C7A-1556FAC92654}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
   </bookViews>
   <sheets>
     <sheet name="reform" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="109">
   <si>
     <t>Folder ID</t>
   </si>
@@ -90,9 +90,6 @@
     <t>dH [MJ/kg]</t>
   </si>
   <si>
-    <t>reform/1</t>
-  </si>
-  <si>
     <t>spec</t>
   </si>
   <si>
@@ -126,33 +123,21 @@
     <t>Run time [min] (cores)</t>
   </si>
   <si>
-    <t>reform/2</t>
-  </si>
-  <si>
     <t>spec,800,600</t>
   </si>
   <si>
     <t>Reform: &gt;May 13</t>
   </si>
   <si>
-    <t>reform/3</t>
-  </si>
-  <si>
     <t>With Darcy, species balance diverge</t>
   </si>
   <si>
     <t>0.0110 (6)</t>
   </si>
   <si>
-    <t>reform/4</t>
-  </si>
-  <si>
     <t>0.0111 (6)</t>
   </si>
   <si>
-    <t>reform/5</t>
-  </si>
-  <si>
     <t>0.0109 (6)</t>
   </si>
   <si>
@@ -165,9 +150,6 @@
     <t>Lower permeability, dense mesh</t>
   </si>
   <si>
-    <t>reform/6</t>
-  </si>
-  <si>
     <t>0.0138 (6)</t>
   </si>
   <si>
@@ -237,18 +219,12 @@
     <t>???</t>
   </si>
   <si>
-    <t>reform/7</t>
-  </si>
-  <si>
     <t>Possible code changes, based on results from Tests\10-12;</t>
   </si>
   <si>
     <t>0.012 (6)</t>
   </si>
   <si>
-    <t>reform/8</t>
-  </si>
-  <si>
     <t>Larger time step from case 7</t>
   </si>
   <si>
@@ -258,30 +234,18 @@
     <t>Case 7, but Cv used for energy advection (GeomClasses); diverges as it reaches end of domain</t>
   </si>
   <si>
-    <t>reform/9</t>
-  </si>
-  <si>
     <t>Lower permeability, Cp of liquid phases;</t>
   </si>
   <si>
-    <t>reform/10</t>
-  </si>
-  <si>
     <t>Even lower permeability, Cp of liq phases;</t>
   </si>
   <si>
-    <t>reform/Ar/1</t>
-  </si>
-  <si>
     <t xml:space="preserve">simulate only Ar as gas (no products); perm calculated from 40 nm particle; </t>
   </si>
   <si>
     <t>0.015 (6)</t>
   </si>
   <si>
-    <t>reform/Ar/2</t>
-  </si>
-  <si>
     <t>0.011 (6)</t>
   </si>
   <si>
@@ -291,12 +255,6 @@
     <t>Ar as gas phase, but advects products Cp;</t>
   </si>
   <si>
-    <t>reform/Ar/3</t>
-  </si>
-  <si>
-    <t>reform/11</t>
-  </si>
-  <si>
     <t>Case 7, but with variable density, proper porosity calc, 40 nm particle;</t>
   </si>
   <si>
@@ -319,9 +277,6 @@
   </si>
   <si>
     <t>Case 11, only solid density into energy source term;</t>
-  </si>
-  <si>
-    <t>reform/12</t>
   </si>
   <si>
     <t>IMPLIED: 40 nm particle diam, eta_ign=0.8, gas_const=107.93, left flux BC, right conv BC</t>
@@ -4489,11 +4444,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B099DE-69DA-496C-8376-9BFCA5F25F37}">
   <dimension ref="A1:U73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U48" sqref="U48"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4518,7 +4473,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>11</v>
@@ -4529,13 +4484,13 @@
         <v>4</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N1" s="4"/>
       <c r="O1" s="1"/>
@@ -4557,7 +4512,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>10</v>
@@ -4566,10 +4521,10 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
         <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
       </c>
       <c r="J2" t="s">
         <v>2</v>
@@ -4581,13 +4536,13 @@
         <v>17</v>
       </c>
       <c r="M2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>6</v>
@@ -4602,7 +4557,7 @@
         <v>16</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>8</v>
@@ -4665,10 +4620,10 @@
         <v>15</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -4728,10 +4683,10 @@
         <v>15</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -4742,7 +4697,7 @@
         <v>3065</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1">
         <v>65</v>
@@ -4793,10 +4748,10 @@
         <v>400000</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -4807,7 +4762,7 @@
         <v>3065</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1">
         <v>65</v>
@@ -4858,10 +4813,10 @@
         <v>140000</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -4872,7 +4827,7 @@
         <v>3065</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D7" s="1">
         <v>65</v>
@@ -4923,21 +4878,19 @@
         <v>200000</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
+      <c r="A8" s="1"/>
       <c r="B8" s="2">
         <v>3065</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1">
         <v>65</v>
@@ -4988,21 +4941,19 @@
         <v>230000</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="B9" s="2">
         <v>3065</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1">
         <v>65</v>
@@ -5053,21 +5004,19 @@
         <v>230000</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
+      <c r="A10" s="1"/>
       <c r="B10" s="2">
         <v>3065</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1">
         <v>65</v>
@@ -5116,10 +5065,10 @@
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -5130,7 +5079,7 @@
         <v>3065</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D11" s="27">
         <v>65</v>
@@ -5179,10 +5128,10 @@
       </c>
       <c r="S11" s="28"/>
       <c r="T11" s="28" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="U11" s="28" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -5193,7 +5142,7 @@
         <v>3065</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D12" s="1">
         <v>65</v>
@@ -5242,10 +5191,10 @@
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -5256,7 +5205,7 @@
         <v>3065</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1">
         <v>65</v>
@@ -5292,7 +5241,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="P13" s="23">
         <v>0.17</v>
@@ -5305,10 +5254,10 @@
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -5332,7 +5281,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -5352,14 +5301,12 @@
       <c r="U15" s="2"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" s="3">
         <v>65</v>
@@ -5406,21 +5353,19 @@
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17" s="3">
         <v>65</v>
@@ -5467,21 +5412,19 @@
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" s="3">
         <v>65</v>
@@ -5528,21 +5471,19 @@
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
       <c r="T18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="U18" s="2" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D19" s="3">
         <v>65</v>
@@ -5589,21 +5530,19 @@
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
       <c r="T19" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A20" s="3"/>
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D20" s="3">
         <v>65</v>
@@ -5650,21 +5589,19 @@
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D21" s="3">
         <v>65</v>
@@ -5709,21 +5646,19 @@
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
       <c r="T21" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="A22" s="3"/>
       <c r="B22" s="2">
         <v>3065</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1">
         <v>65</v>
@@ -5774,10 +5709,10 @@
         <v>400000</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -5785,7 +5720,7 @@
         <v>3065</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D23" s="1">
         <v>65</v>
@@ -5832,21 +5767,19 @@
       <c r="R23" s="2"/>
       <c r="S23" s="12"/>
       <c r="T23" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="A24" s="3"/>
       <c r="B24" s="2">
         <v>3065</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1">
         <v>65</v>
@@ -5895,21 +5828,19 @@
       </c>
       <c r="S24" s="12"/>
       <c r="T24" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>74</v>
-      </c>
+      <c r="A25" s="3"/>
       <c r="B25" s="2">
         <v>3065</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1">
         <v>65</v>
@@ -5958,21 +5889,19 @@
       </c>
       <c r="S25" s="12"/>
       <c r="T25" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="A26" s="3"/>
       <c r="B26" s="2">
         <v>3065</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D26" s="1">
         <v>65</v>
@@ -6021,21 +5950,19 @@
       </c>
       <c r="S26" s="9"/>
       <c r="T26" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="A27" s="3"/>
       <c r="B27" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D27" s="1">
         <v>65</v>
@@ -6085,18 +6012,16 @@
       <c r="S27" s="9"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>95</v>
-      </c>
+      <c r="A28" s="3"/>
       <c r="B28" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D28" s="1">
         <v>65</v>
@@ -6145,10 +6070,10 @@
       </c>
       <c r="S28" s="9"/>
       <c r="T28" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="U28" s="2" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -6198,14 +6123,12 @@
       <c r="U30" s="2"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="A31" s="3"/>
       <c r="B31" s="2">
         <v>2043</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D31" s="1">
         <v>65</v>
@@ -6254,21 +6177,19 @@
       </c>
       <c r="S31" s="12"/>
       <c r="T31" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="A32" s="3"/>
       <c r="B32" s="2">
         <v>2043</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D32" s="1">
         <v>65</v>
@@ -6317,21 +6238,19 @@
       </c>
       <c r="S32" s="12"/>
       <c r="T32" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="A33" s="3"/>
       <c r="B33" s="2">
         <v>2043</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D33" s="1">
         <v>65</v>
@@ -6375,7 +6294,7 @@
       <c r="S33" s="12"/>
       <c r="T33" s="2"/>
       <c r="U33" s="9" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -6403,7 +6322,7 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -6413,7 +6332,7 @@
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
       <c r="I35" s="34" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="12"/>
@@ -6430,13 +6349,13 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B36" s="2">
         <v>5109</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D36" s="1">
         <v>65</v>
@@ -6483,21 +6402,21 @@
       <c r="R36" s="9"/>
       <c r="S36" s="9"/>
       <c r="T36" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="U36" s="9" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D37" s="1">
         <v>65</v>
@@ -6542,21 +6461,21 @@
       <c r="R37" s="9"/>
       <c r="S37" s="9"/>
       <c r="T37" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="U37" s="9" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D38" s="1">
         <v>65</v>
@@ -6603,21 +6522,21 @@
       <c r="R38" s="9"/>
       <c r="S38" s="12"/>
       <c r="T38" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="U38" s="2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D39" s="1">
         <v>65</v>
@@ -6664,21 +6583,21 @@
       <c r="R39" s="9"/>
       <c r="S39" s="12"/>
       <c r="T39" s="9" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="U39" s="2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D40" s="1">
         <v>65</v>
@@ -6725,21 +6644,21 @@
       <c r="R40" s="9"/>
       <c r="S40" s="12"/>
       <c r="T40" s="9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D41" s="1">
         <v>65</v>
@@ -6786,10 +6705,10 @@
       <c r="R41" s="9"/>
       <c r="S41" s="12"/>
       <c r="T41" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="U41" s="2" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -6817,7 +6736,7 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -6842,13 +6761,13 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="B44" s="2">
         <v>5109</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D44" s="1">
         <v>65</v>
@@ -6890,18 +6809,18 @@
       <c r="S44" s="12"/>
       <c r="T44" s="9"/>
       <c r="U44" s="9" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D45" s="1">
         <v>65</v>
@@ -6943,18 +6862,18 @@
       <c r="S45" s="12"/>
       <c r="T45" s="9"/>
       <c r="U45" s="9" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D46" s="1">
         <v>65</v>
@@ -6996,18 +6915,18 @@
       <c r="S46" s="12"/>
       <c r="T46" s="9"/>
       <c r="U46" s="2" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D47" s="1">
         <v>65</v>
@@ -7054,21 +6973,21 @@
       <c r="R47" s="9"/>
       <c r="S47" s="12"/>
       <c r="T47" s="9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="U47" s="2" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D48" s="1">
         <v>65</v>
@@ -7115,21 +7034,21 @@
       </c>
       <c r="S48" s="9"/>
       <c r="T48" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="U48" s="2" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D49" s="1">
         <v>65</v>
@@ -7176,10 +7095,10 @@
       <c r="R49" s="9"/>
       <c r="S49" s="12"/>
       <c r="T49" s="9" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
@@ -7704,7 +7623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6D8385-D5DE-4DEC-BF2A-2B2794E481A2}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -7712,23 +7631,23 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -7821,7 +7740,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>

</xml_diff>

<commit_message>
Misc: Sync Nov 24
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\1D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C62B0D6-2DF2-4644-B0B8-1DABE0E8B856}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0A646F-F65D-4315-AB32-F4B9B90392BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
+    <workbookView xWindow="17355" yWindow="4395" windowWidth="21600" windowHeight="11385" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
   </bookViews>
   <sheets>
     <sheet name="reform" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="164">
   <si>
     <t>Folder ID</t>
   </si>
@@ -433,9 +433,6 @@
     <t>nano/40nm_gasgen/6</t>
   </si>
   <si>
-    <t>NOTES: Using Cv of air for gaseous species state, rhoC implementation, Cp of molten species (998)</t>
-  </si>
-  <si>
     <t>Ignition</t>
   </si>
   <si>
@@ -503,6 +500,33 @@
   </si>
   <si>
     <t>Same as 1 but Cv maxed at 3000K; smaller oscillations</t>
+  </si>
+  <si>
+    <t>Same as 1 but Air at 1000K (Cv), variable porosity/perm; wave at end of domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTES: Using Cv of air at 1000 K for gas species, rhoC implementation, Cp of air at T, gas_gen:0.343, variable porosity/perm, </t>
+  </si>
+  <si>
+    <t>Wave at end of domain</t>
+  </si>
+  <si>
+    <t>nano/40nm_gasgen/6a</t>
+  </si>
+  <si>
+    <t>Used O2 for gas specie instead</t>
+  </si>
+  <si>
+    <t>nano/40nm_gasgen/6b</t>
+  </si>
+  <si>
+    <t>10 times Carmen_diam; wave at end of domain, some instabilities after ignition; final time step 10^-11</t>
+  </si>
+  <si>
+    <t>nano/40nm_gasgen/6P</t>
+  </si>
+  <si>
+    <t>0 pressure BCs</t>
   </si>
 </sst>
 </file>
@@ -6766,13 +6790,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B099DE-69DA-496C-8376-9BFCA5F25F37}">
-  <dimension ref="A1:U88"/>
+  <dimension ref="A1:U92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="R63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="M69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U82" sqref="U82"/>
+      <selection pane="bottomRight" activeCell="P77" sqref="P77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10061,7 +10085,7 @@
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -10089,12 +10113,12 @@
       <c r="S62" s="12"/>
       <c r="T62" s="9"/>
       <c r="U62" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -10122,12 +10146,12 @@
       <c r="S63" s="12"/>
       <c r="T63" s="9"/>
       <c r="U63" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -10155,12 +10179,12 @@
       <c r="S64" s="12"/>
       <c r="T64" s="9"/>
       <c r="U64" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -10188,12 +10212,12 @@
       <c r="S65" s="12"/>
       <c r="T65" s="9"/>
       <c r="U65" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -10221,7 +10245,7 @@
       <c r="S66" s="12"/>
       <c r="T66" s="9"/>
       <c r="U66" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
@@ -10274,7 +10298,7 @@
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -10342,10 +10366,10 @@
       </c>
       <c r="O70" s="5"/>
       <c r="P70" s="20">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="Q70" s="20">
-        <v>1.9</v>
+        <v>3.7</v>
       </c>
       <c r="R70" s="9"/>
       <c r="S70" s="9"/>
@@ -10396,12 +10420,8 @@
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="O71" s="5"/>
-      <c r="P71" s="20">
-        <v>0.38</v>
-      </c>
-      <c r="Q71" s="20">
-        <v>2.36</v>
-      </c>
+      <c r="P71" s="20"/>
+      <c r="Q71" s="20"/>
       <c r="R71" s="9"/>
       <c r="S71" s="12"/>
       <c r="T71" s="9"/>
@@ -10451,12 +10471,8 @@
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="O72" s="5"/>
-      <c r="P72" s="20">
-        <v>0.32</v>
-      </c>
-      <c r="Q72" s="20">
-        <v>3.47</v>
-      </c>
+      <c r="P72" s="20"/>
+      <c r="Q72" s="20"/>
       <c r="R72" s="9"/>
       <c r="S72" s="9"/>
       <c r="T72" s="9"/>
@@ -10506,12 +10522,8 @@
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="O73" s="5"/>
-      <c r="P73" s="20">
-        <v>0.25</v>
-      </c>
-      <c r="Q73" s="20">
-        <v>5.1100000000000003</v>
-      </c>
+      <c r="P73" s="20"/>
+      <c r="Q73" s="20"/>
       <c r="R73" s="9"/>
       <c r="S73" s="9"/>
       <c r="T73" s="9"/>
@@ -10561,12 +10573,8 @@
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="O74" s="5"/>
-      <c r="P74" s="20">
-        <v>0.16</v>
-      </c>
-      <c r="Q74" s="20">
-        <v>6.59</v>
-      </c>
+      <c r="P74" s="20"/>
+      <c r="Q74" s="20"/>
       <c r="R74" s="9"/>
       <c r="S74" s="12"/>
       <c r="T74" s="9"/>
@@ -10615,69 +10623,145 @@
       <c r="N75" s="11">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="O75" s="5"/>
+      <c r="O75" s="17">
+        <v>1463395</v>
+      </c>
       <c r="P75" s="20">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="Q75" s="20">
-        <v>6.03</v>
+        <v>57.85</v>
       </c>
       <c r="R75" s="9"/>
       <c r="S75" s="9"/>
-      <c r="T75" s="9"/>
-      <c r="U75" s="9"/>
+      <c r="T75" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="U75" s="9" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="9"/>
-      <c r="J76" s="2"/>
-      <c r="K76" s="2"/>
-      <c r="L76" s="2"/>
-      <c r="M76" s="15"/>
-      <c r="N76" s="2"/>
-      <c r="O76" s="3"/>
-      <c r="P76" s="20"/>
-      <c r="Q76" s="20"/>
+      <c r="A76" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D76" s="1">
+        <v>65</v>
+      </c>
+      <c r="E76" s="2">
+        <v>3</v>
+      </c>
+      <c r="F76" s="2">
+        <v>600</v>
+      </c>
+      <c r="G76" s="2">
+        <v>200</v>
+      </c>
+      <c r="H76" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I76" s="36">
+        <v>0.9</v>
+      </c>
+      <c r="J76" s="2">
+        <v>48</v>
+      </c>
+      <c r="K76" s="22">
+        <v>4890000</v>
+      </c>
+      <c r="L76" s="23">
+        <v>2.78</v>
+      </c>
+      <c r="M76" s="16">
+        <v>1E-10</v>
+      </c>
+      <c r="N76" s="11">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="O76" s="17">
+        <v>2204804</v>
+      </c>
+      <c r="P76" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="Q76" s="20">
+        <v>19.670000000000002</v>
+      </c>
       <c r="R76" s="9"/>
       <c r="S76" s="9"/>
       <c r="T76" s="9"/>
-      <c r="U76" s="9"/>
+      <c r="U76" s="9" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9"/>
-      <c r="J77" s="2"/>
-      <c r="K77" s="11"/>
-      <c r="L77" s="11"/>
-      <c r="M77" s="16"/>
-      <c r="N77" s="11"/>
-      <c r="O77" s="3"/>
-      <c r="P77" s="18"/>
-      <c r="Q77" s="18"/>
-      <c r="R77" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D77" s="1">
+        <v>65</v>
+      </c>
+      <c r="E77" s="2">
+        <v>3</v>
+      </c>
+      <c r="F77" s="2">
+        <v>600</v>
+      </c>
+      <c r="G77" s="2">
+        <v>200</v>
+      </c>
+      <c r="H77" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I77" s="36">
+        <v>0.9</v>
+      </c>
+      <c r="J77" s="2">
+        <v>48</v>
+      </c>
+      <c r="K77" s="22">
+        <v>4890000</v>
+      </c>
+      <c r="L77" s="23">
+        <v>2.78</v>
+      </c>
+      <c r="M77" s="16">
+        <v>1E-10</v>
+      </c>
+      <c r="N77" s="11">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="O77" s="17"/>
+      <c r="P77" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="Q77" s="20">
+        <v>145.27000000000001</v>
+      </c>
+      <c r="R77" s="9"/>
       <c r="S77" s="9"/>
-      <c r="T77" s="9"/>
-      <c r="U77" s="9"/>
+      <c r="T77" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="U77" s="9" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A78" s="3">
-        <v>1</v>
+      <c r="A78" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>18</v>
@@ -10701,7 +10785,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="I78" s="36">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="J78" s="2">
         <v>48</v>
@@ -10716,114 +10800,126 @@
         <v>1E-10</v>
       </c>
       <c r="N78" s="11">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="O78" s="3"/>
-      <c r="P78" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="Q78" s="20">
-        <v>4.24</v>
-      </c>
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="O78" s="17"/>
+      <c r="P78" s="20"/>
+      <c r="Q78" s="20"/>
       <c r="R78" s="9"/>
       <c r="S78" s="9"/>
       <c r="T78" s="9"/>
       <c r="U78" s="9" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A79" s="3">
-        <v>2</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D79" s="1">
-        <v>65</v>
-      </c>
-      <c r="E79" s="2">
-        <v>3</v>
-      </c>
-      <c r="F79" s="2">
-        <v>600</v>
-      </c>
-      <c r="G79" s="2">
-        <v>200</v>
-      </c>
-      <c r="H79" s="25">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="I79" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="J79" s="2">
-        <v>48</v>
-      </c>
-      <c r="K79" s="22">
-        <v>4890000</v>
-      </c>
-      <c r="L79" s="23">
-        <v>2.78</v>
-      </c>
-      <c r="M79" s="16">
-        <v>1E-10</v>
-      </c>
-      <c r="N79" s="11">
-        <v>2.9999999999999997E-4</v>
-      </c>
+      <c r="A79" s="6"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="2"/>
       <c r="O79" s="3"/>
-      <c r="P79" s="20">
-        <v>0.15</v>
-      </c>
-      <c r="Q79" s="20">
-        <v>7.11</v>
-      </c>
+      <c r="P79" s="20"/>
+      <c r="Q79" s="20"/>
       <c r="R79" s="9"/>
       <c r="S79" s="9"/>
       <c r="T79" s="9"/>
-      <c r="U79" s="9" t="s">
-        <v>141</v>
-      </c>
+      <c r="U79" s="9"/>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="4"/>
-      <c r="J80" s="4"/>
-      <c r="K80" s="4"/>
-      <c r="L80" s="4"/>
-      <c r="M80" s="14"/>
-      <c r="N80" s="4"/>
-      <c r="O80" s="1"/>
-      <c r="P80" s="21"/>
-      <c r="Q80" s="21"/>
+      <c r="A80" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="11"/>
+      <c r="L80" s="11"/>
+      <c r="M80" s="16"/>
+      <c r="N80" s="11"/>
+      <c r="O80" s="3"/>
+      <c r="P80" s="18"/>
+      <c r="Q80" s="18"/>
+      <c r="R80" s="2"/>
+      <c r="S80" s="9"/>
+      <c r="T80" s="9"/>
+      <c r="U80" s="9"/>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="4"/>
-      <c r="J81" s="4"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-      <c r="M81" s="14"/>
-      <c r="N81" s="4"/>
-      <c r="O81" s="1"/>
-      <c r="P81" s="21"/>
-      <c r="Q81" s="21"/>
+      <c r="A81" s="3">
+        <v>1</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D81" s="1">
+        <v>65</v>
+      </c>
+      <c r="E81" s="2">
+        <v>3</v>
+      </c>
+      <c r="F81" s="2">
+        <v>600</v>
+      </c>
+      <c r="G81" s="2">
+        <v>200</v>
+      </c>
+      <c r="H81" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I81" s="36">
+        <v>0.4</v>
+      </c>
+      <c r="J81" s="2">
+        <v>48</v>
+      </c>
+      <c r="K81" s="22">
+        <v>4890000</v>
+      </c>
+      <c r="L81" s="23">
+        <v>2.78</v>
+      </c>
+      <c r="M81" s="16">
+        <v>1E-10</v>
+      </c>
+      <c r="N81" s="11">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="O81" s="3"/>
+      <c r="P81" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="Q81" s="20">
+        <v>4.24</v>
+      </c>
+      <c r="R81" s="9"/>
+      <c r="S81" s="9"/>
+      <c r="T81" s="9"/>
+      <c r="U81" s="9" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <v>1</v>
+      <c r="A82" s="3">
+        <v>2</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>18</v>
@@ -10847,7 +10943,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="I82" s="36">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="J82" s="2">
         <v>48</v>
@@ -10859,172 +10955,168 @@
         <v>2.78</v>
       </c>
       <c r="M82" s="16">
-        <v>5.0000000000000002E-11</v>
+        <v>1E-10</v>
       </c>
       <c r="N82" s="11">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="O82" s="1"/>
-      <c r="P82" s="21">
+      <c r="O82" s="3"/>
+      <c r="P82" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="Q82" s="20">
+        <v>7.11</v>
+      </c>
+      <c r="R82" s="9"/>
+      <c r="S82" s="9"/>
+      <c r="T82" s="9"/>
+      <c r="U82" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="4"/>
+      <c r="J83" s="4"/>
+      <c r="K83" s="4"/>
+      <c r="L83" s="4"/>
+      <c r="M83" s="14"/>
+      <c r="N83" s="4"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="21"/>
+      <c r="Q83" s="21"/>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="4"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="14"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="21"/>
+      <c r="Q84" s="21"/>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>1</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D85" s="1">
+        <v>65</v>
+      </c>
+      <c r="E85" s="2">
+        <v>3</v>
+      </c>
+      <c r="F85" s="2">
+        <v>600</v>
+      </c>
+      <c r="G85" s="2">
+        <v>200</v>
+      </c>
+      <c r="H85" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I85" s="36">
+        <v>0.6</v>
+      </c>
+      <c r="J85" s="2">
+        <v>48</v>
+      </c>
+      <c r="K85" s="22">
+        <v>4890000</v>
+      </c>
+      <c r="L85" s="23">
+        <v>2.78</v>
+      </c>
+      <c r="M85" s="16">
+        <v>5.0000000000000002E-11</v>
+      </c>
+      <c r="N85" s="11">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="O85" s="1"/>
+      <c r="P85" s="21">
         <v>0.23</v>
       </c>
-      <c r="Q82" s="21">
+      <c r="Q85" s="21">
         <v>10.1</v>
       </c>
-      <c r="U82" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+      <c r="U85" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
         <v>2</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D83" s="1">
+      <c r="D86" s="1">
         <v>65</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E86" s="2">
         <v>3</v>
       </c>
-      <c r="F83" s="2">
+      <c r="F86" s="2">
         <v>600</v>
       </c>
-      <c r="G83" s="2">
+      <c r="G86" s="2">
         <v>200</v>
       </c>
-      <c r="H83" s="25">
+      <c r="H86" s="25">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="I83" s="36">
+      <c r="I86" s="36">
         <v>0.6</v>
       </c>
-      <c r="J83" s="2">
+      <c r="J86" s="2">
         <v>48</v>
       </c>
-      <c r="K83" s="22">
+      <c r="K86" s="22">
         <v>4890000</v>
       </c>
-      <c r="L83" s="23">
+      <c r="L86" s="23">
         <v>2.78</v>
       </c>
-      <c r="M83" s="16">
+      <c r="M86" s="16">
         <v>1E-10</v>
       </c>
-      <c r="N83" s="11">
+      <c r="N86" s="11">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="O83" s="1"/>
-      <c r="P83" s="21">
+      <c r="O86" s="1"/>
+      <c r="P86" s="21">
         <v>0.23</v>
       </c>
-      <c r="Q83" s="21">
+      <c r="Q86" s="21">
         <v>22.53</v>
       </c>
-      <c r="U83" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A84" s="39" t="s">
+      <c r="U86" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A87" s="39" t="s">
         <v>111</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D84" s="1">
-        <v>65</v>
-      </c>
-      <c r="E84" s="2">
-        <v>3</v>
-      </c>
-      <c r="F84" s="2">
-        <v>600</v>
-      </c>
-      <c r="G84" s="2">
-        <v>200</v>
-      </c>
-      <c r="H84" s="25">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="I84" s="36">
-        <v>0.6</v>
-      </c>
-      <c r="J84" s="2">
-        <v>48</v>
-      </c>
-      <c r="K84" s="22">
-        <v>4890000</v>
-      </c>
-      <c r="L84" s="23">
-        <v>2.78</v>
-      </c>
-      <c r="M84" s="16">
-        <v>1E-10</v>
-      </c>
-      <c r="N84" s="11">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="O84" s="1"/>
-      <c r="P84" s="21">
-        <v>0.23</v>
-      </c>
-      <c r="Q84" s="21">
-        <v>9.09</v>
-      </c>
-      <c r="T84" t="s">
-        <v>154</v>
-      </c>
-      <c r="U84" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="25"/>
-      <c r="I85" s="36"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="22"/>
-      <c r="L85" s="23"/>
-      <c r="M85" s="16"/>
-      <c r="N85" s="11"/>
-      <c r="O85" s="1"/>
-      <c r="P85" s="21"/>
-      <c r="Q85" s="21"/>
-    </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="4"/>
-      <c r="J86" s="4"/>
-      <c r="K86" s="4"/>
-      <c r="L86" s="4"/>
-      <c r="M86" s="14"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="1"/>
-      <c r="P86" s="21"/>
-      <c r="Q86" s="21"/>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>1</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>18</v>
@@ -11048,7 +11140,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="I87" s="36">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="J87" s="2">
         <v>48</v>
@@ -11066,19 +11158,22 @@
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="O87" s="1"/>
-      <c r="P87" s="23">
-        <v>0.15</v>
-      </c>
-      <c r="Q87" s="23">
-        <v>7.11</v>
+      <c r="P87" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="Q87" s="21">
+        <v>9.09</v>
+      </c>
+      <c r="T87" t="s">
+        <v>153</v>
       </c>
       <c r="U87" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>2</v>
+      <c r="A88" s="39">
+        <v>3</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>18</v>
@@ -11116,20 +11211,167 @@
       <c r="M88" s="16">
         <v>1E-10</v>
       </c>
-      <c r="N88" s="11">
-        <v>2.9999999999999997E-4</v>
-      </c>
+      <c r="N88" s="38">
+        <v>2.9700000000000001E-4</v>
+      </c>
+      <c r="O88" s="1"/>
       <c r="P88" s="21">
         <v>0.23</v>
       </c>
       <c r="Q88" s="21">
+        <v>42.71</v>
+      </c>
+      <c r="T88" t="s">
+        <v>55</v>
+      </c>
+      <c r="U88" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="25"/>
+      <c r="I89" s="36"/>
+      <c r="J89" s="2"/>
+      <c r="K89" s="22"/>
+      <c r="L89" s="23"/>
+      <c r="M89" s="16"/>
+      <c r="N89" s="11"/>
+      <c r="O89" s="1"/>
+      <c r="P89" s="21"/>
+      <c r="Q89" s="21"/>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+      <c r="M90" s="14"/>
+      <c r="N90" s="4"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="21"/>
+      <c r="Q90" s="21"/>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D91" s="1">
+        <v>65</v>
+      </c>
+      <c r="E91" s="2">
+        <v>3</v>
+      </c>
+      <c r="F91" s="2">
+        <v>600</v>
+      </c>
+      <c r="G91" s="2">
+        <v>200</v>
+      </c>
+      <c r="H91" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I91" s="36">
+        <v>0.8</v>
+      </c>
+      <c r="J91" s="2">
+        <v>48</v>
+      </c>
+      <c r="K91" s="22">
+        <v>4890000</v>
+      </c>
+      <c r="L91" s="23">
+        <v>2.78</v>
+      </c>
+      <c r="M91" s="16">
+        <v>1E-10</v>
+      </c>
+      <c r="N91" s="11">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="O91" s="1"/>
+      <c r="P91" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="Q91" s="23">
+        <v>7.11</v>
+      </c>
+      <c r="U91" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>2</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D92" s="1">
+        <v>65</v>
+      </c>
+      <c r="E92" s="2">
+        <v>3</v>
+      </c>
+      <c r="F92" s="2">
+        <v>600</v>
+      </c>
+      <c r="G92" s="2">
+        <v>200</v>
+      </c>
+      <c r="H92" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I92" s="36">
+        <v>0.6</v>
+      </c>
+      <c r="J92" s="2">
+        <v>48</v>
+      </c>
+      <c r="K92" s="22">
+        <v>4890000</v>
+      </c>
+      <c r="L92" s="23">
+        <v>2.78</v>
+      </c>
+      <c r="M92" s="16">
+        <v>1E-10</v>
+      </c>
+      <c r="N92" s="11">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="P92" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="Q92" s="21">
         <v>5.78</v>
       </c>
-      <c r="T88" t="s">
-        <v>154</v>
-      </c>
-      <c r="U88" t="s">
+      <c r="T92" t="s">
         <v>153</v>
+      </c>
+      <c r="U92" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -11364,10 +11606,10 @@
         <v>89</v>
       </c>
       <c r="B20" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>133</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>